<commit_message>
Update Optica BAC-06-Catálogo de componentes.xlsx
</commit_message>
<xml_diff>
--- a/HT-4/Optica BAC-06-Catálogo de componentes.xlsx
+++ b/HT-4/Optica BAC-06-Catálogo de componentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvill\Dropbox\uniandes\MATI\Notas de clase\Artefactos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179E59CC-F15C-4395-9FE3-2F8856D9905A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7871F6-E53C-4E42-876B-9046C7D1015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="525" windowWidth="17445" windowHeight="14910" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="28800" yWindow="-5900" windowWidth="38400" windowHeight="21100" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-06" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Nombre</t>
   </si>
@@ -55,6 +55,63 @@
   </si>
   <si>
     <t>Modelo de negocio</t>
+  </si>
+  <si>
+    <t>Proveedor lentes</t>
+  </si>
+  <si>
+    <t>Proveedor monturas</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Montura</t>
+  </si>
+  <si>
+    <t>Montura con lentes</t>
+  </si>
+  <si>
+    <t>Información</t>
+  </si>
+  <si>
+    <t>Dinero</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Empresa a la que se le compran los lentes formulados o con modificaciones</t>
+  </si>
+  <si>
+    <t>Empresa a la que se le compran las monturas</t>
+  </si>
+  <si>
+    <t>Persona compradora de los productos y servicios de la óptica</t>
+  </si>
+  <si>
+    <t>Persona que necesita un examen ocular para saber la corrección que debe tener en sus ojos</t>
+  </si>
+  <si>
+    <t>Estructura, generalmente de plástico o metal, que sostiene los lentes y reposa sobre la nariz y las orejas</t>
+  </si>
+  <si>
+    <t>Estructura, generalmente de plástico o metal, que sostiene los lentes y reposa sobre la nariz y las orejas. Los lentes son vidrios transparentes utilizados para la corrección de la visión.</t>
+  </si>
+  <si>
+    <t>Lentes</t>
+  </si>
+  <si>
+    <t>Monturas</t>
+  </si>
+  <si>
+    <t>Productos comprados</t>
+  </si>
+  <si>
+    <t>Servicios adquiridos</t>
   </si>
 </sst>
 </file>
@@ -96,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -119,20 +176,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -152,7 +270,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -448,102 +566,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="12.875" customWidth="1"/>
-    <col min="4" max="4" width="29.625" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
+    <row r="6" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" customFormat="1" ht="60" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" customFormat="1" ht="90" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="1:4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="1:4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="1:4" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="1:4" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>